<commit_message>
Printing 4 prop guard covers
</commit_message>
<xml_diff>
--- a/Print Specs.xlsx
+++ b/Print Specs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilyas\Desktop\Quad Squad\Mechanical\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Quadcopter System Solutions\Mechanical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A149FE-E484-4BD3-A9D8-66F840E216DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2351A6F7-CFBC-49AA-B741-E0A2044C78EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Infill %</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>QUAD SQUAD PRINT DATA</t>
+  </si>
+  <si>
+    <t>11g</t>
   </si>
 </sst>
 </file>
@@ -137,14 +140,16 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -425,70 +430,70 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1"/>
-    <col min="6" max="6" width="18.77734375" customWidth="1"/>
-    <col min="7" max="7" width="22.5546875" customWidth="1"/>
-    <col min="8" max="8" width="26.44140625" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" customWidth="1"/>
-    <col min="10" max="10" width="10.88671875" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -513,7 +518,9 @@
       <c r="H3" s="4">
         <v>0.4</v>
       </c>
-      <c r="I3" s="4"/>
+      <c r="I3" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="J3" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
infill test print and P1 arm started
</commit_message>
<xml_diff>
--- a/Print Specs.xlsx
+++ b/Print Specs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilyas\Desktop\Quad Squad\Mechanical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC979C9-EBDD-47F2-984F-58D2CF349013}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486BA20B-07FF-4DCD-9128-55DE86D11DDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Infill %</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>P0 Cover</t>
+  </si>
+  <si>
+    <t>P1 arm infill test</t>
+  </si>
+  <si>
+    <t>3D cubic</t>
+  </si>
+  <si>
+    <t>3D honeycomb</t>
+  </si>
+  <si>
+    <t>triangles (3d?)</t>
   </si>
 </sst>
 </file>
@@ -140,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -150,9 +162,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -433,17 +444,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.88671875" customWidth="1"/>
     <col min="3" max="3" width="16.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.88671875" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" customWidth="1"/>
     <col min="7" max="7" width="22.5546875" customWidth="1"/>
@@ -530,30 +542,118 @@
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>0.2</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3">
         <v>5</v>
       </c>
-      <c r="F4" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
+      <c r="F4" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3">
+        <v>25</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3">
+        <v>25</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="3">
+        <v>25</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>